<commit_message>
Embed external files into assembly file
Create and use new bespoke factory class BitmapImageFactory and Streams
to embed files into the assembly file and allow the code to run on
different machines.
</commit_message>
<xml_diff>
--- a/TestExcelFiles/ColumnNameRevitVSEtabs.xlsx
+++ b/TestExcelFiles/ColumnNameRevitVSEtabs.xlsx
@@ -1405,4 +1405,275 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF8DE7CCB26837419550FEA72B4C2D38" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="66e49ef64fc7c6fc6c8bd2849f7fe18b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9f9fa968-25b7-469f-b458-273e8c5fa4fe" xmlns:ns3="7c910a83-52a8-41c3-bcfc-89f30461189b" xmlns:ns4="8f7a92c5-f891-48be-92b1-40f67a03cf11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6824ea96a3c0cc3629e5764cc647c496" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="9f9fa968-25b7-469f-b458-273e8c5fa4fe"/>
+    <xsd:import namespace="7c910a83-52a8-41c3-bcfc-89f30461189b"/>
+    <xsd:import namespace="8f7a92c5-f891-48be-92b1-40f67a03cf11"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9f9fa968-25b7-469f-b458-273e8c5fa4fe" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="18" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="43fa978b-cdad-45a5-877c-f631a0e6dfe9" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="22" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7c910a83-52a8-41c3-bcfc-89f30461189b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8f7a92c5-f891-48be-92b1-40f67a03cf11" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="19" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{0f4d1250-dd80-4a3f-be63-7b20a0463b4f}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7c910a83-52a8-41c3-bcfc-89f30461189b">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A3388A8-0841-4ABF-919F-3F4D61CA996B}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D2300E8-734F-428C-A230-9D2812FD421C}"/>
 </file>
</xml_diff>